<commit_message>
Backup + Report start
</commit_message>
<xml_diff>
--- a/src/experiments/experiment_results.xlsx
+++ b/src/experiments/experiment_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
   <si>
     <t xml:space="preserve">BOHB</t>
   </si>
@@ -145,12 +145,21 @@
     <t xml:space="preserve">BOHB_KMNIST_2_1_16</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show learning curve</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model:               </t>
   </si>
   <si>
     <t xml:space="preserve">BOHB_KMNIST_3_1_9</t>
   </si>
   <si>
+    <t xml:space="preserve">Did the test loss actually decrease for K49</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model name:          </t>
   </si>
   <si>
@@ -160,6 +169,9 @@
     <t xml:space="preserve">BOHB_KMNIST_4_1_16</t>
   </si>
   <si>
+    <t xml:space="preserve">Did it really learn?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stepping:            </t>
   </si>
   <si>
@@ -214,10 +226,22 @@
     <t xml:space="preserve">6144K</t>
   </si>
   <si>
+    <t xml:space="preserve">BOHB_KMNIST_3_2_20 (Subsetted data)</t>
+  </si>
+  <si>
     <t xml:space="preserve">NUMA node0 CPU(s):   </t>
   </si>
   <si>
     <t xml:space="preserve">`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default: K49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Epochs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default: KMNIST</t>
   </si>
 </sst>
 </file>
@@ -228,7 +252,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -267,6 +291,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCE181E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -339,8 +370,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -359,12 +390,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -376,6 +407,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -384,10 +475,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+      <selection pane="topLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,7 +594,7 @@
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -556,7 +647,7 @@
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -606,7 +697,7 @@
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -653,10 +744,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="8" t="n">
@@ -703,10 +794,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -753,423 +844,375 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R9" s="0" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R10" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="S9" s="0" t="n">
+      <c r="S10" s="0" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R10" s="0" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R12" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="S10" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R11" s="0" t="s">
+      <c r="S12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R13" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="S11" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="S13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="R12" s="0" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="R14" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="S12" s="0" t="s">
+      <c r="S14" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="R13" s="0" t="s">
+      <c r="R15" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="S13" s="0" t="n">
+      <c r="S15" s="0" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D16" s="7" t="n">
         <v>0.9958</v>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="E16" s="7" t="n">
         <v>0.9469</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G14" s="0" t="s">
+      <c r="F16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H16" s="7" t="n">
         <v>0.9645</v>
       </c>
-      <c r="I14" s="7" t="n">
+      <c r="I16" s="7" t="n">
         <v>0.8991</v>
       </c>
-      <c r="J14" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="K14" s="0" t="n">
+      <c r="J16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K16" s="0" t="n">
         <f aca="false">447.788898229599+1695.3580596447</f>
         <v>2143.1469578743</v>
       </c>
-      <c r="R14" s="0" t="s">
+      <c r="L16" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="S14" s="0" t="n">
+      <c r="M16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="S16" s="0" t="n">
         <v>142</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="0" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D17" s="7" t="n">
         <v>0.9823</v>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="E17" s="7" t="n">
         <v>0.9326</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F17" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H17" s="7" t="n">
         <v>0.9326</v>
       </c>
-      <c r="I15" s="7" t="n">
+      <c r="I17" s="7" t="n">
         <v>0.8605</v>
       </c>
-      <c r="J15" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="K15" s="0" t="n">
+      <c r="J17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K17" s="0" t="n">
         <f aca="false">474.691176652908+3283.0042052269</f>
         <v>3757.69538187981</v>
       </c>
-      <c r="R15" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="S15" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="M17" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="R17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D18" s="7" t="n">
         <v>0.9995</v>
       </c>
-      <c r="E16" s="7" t="n">
+      <c r="E18" s="7" t="n">
         <v>0.9598</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F18" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="7" t="n">
+      <c r="H18" s="7" t="n">
         <v>0.9963</v>
       </c>
-      <c r="I16" s="7" t="n">
+      <c r="I18" s="7" t="n">
         <v>0.9307</v>
       </c>
-      <c r="J16" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="K16" s="0" t="n">
+      <c r="J18" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K18" s="0" t="n">
         <f aca="false">1109.43264222145+6734.84380841255</f>
         <v>7844.276450634</v>
       </c>
-      <c r="R16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="S16" s="0" t="n">
+      <c r="M18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="S18" s="0" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="0" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D19" s="7" t="n">
         <v>0.9956</v>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E19" s="7" t="n">
         <v>0.953</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="F19" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="7" t="n">
+      <c r="H19" s="7" t="n">
         <v>0.97</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I19" s="7" t="n">
         <v>0.92</v>
       </c>
-      <c r="J17" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="K17" s="0" t="n">
+      <c r="J19" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K19" s="0" t="n">
         <f aca="false">237.180494070053+1001.07636117935</f>
         <v>1238.2568552494</v>
       </c>
-      <c r="R17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="S17" s="0" t="n">
+      <c r="R19" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="S19" s="0" t="n">
         <v>2873.017</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="0" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D20" s="7" t="n">
         <v>0.9855</v>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="E20" s="7" t="n">
         <v>0.8778</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F20" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G20" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="7" t="n">
-        <v>0.9998</v>
-      </c>
-      <c r="I18" s="7" t="n">
+      <c r="H20" s="7" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="I20" s="7" t="n">
         <v>0.943</v>
       </c>
-      <c r="J18" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="K18" s="0" t="n">
+      <c r="J20" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K20" s="0" t="n">
         <f aca="false">860.058214664459+750.98587179184</f>
         <v>1611.0440864563</v>
       </c>
-      <c r="R18" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="S18" s="0" t="n">
+      <c r="R20" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="S20" s="0" t="n">
         <v>3400</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R19" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="S19" s="0" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R20" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="S20" s="0" t="n">
-        <v>3600</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="R21" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="S21" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="S21" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="R22" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="S22" s="0" t="s">
+      <c r="S22" s="0" t="n">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R23" s="0" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R23" s="0" t="s">
+      <c r="S23" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="S23" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <v>13888.2287483215</v>
-      </c>
-      <c r="I24" s="7" t="n">
-        <v>0.9817</v>
-      </c>
-      <c r="J24" s="7" t="n">
-        <v>0.9609</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="L24" s="7" t="n">
-        <v>0.9887</v>
-      </c>
-      <c r="M24" s="7" t="n">
-        <v>0.902</v>
-      </c>
-      <c r="N24" s="0" t="n">
-        <v>20</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
       <c r="R24" s="0" t="s">
         <v>60</v>
       </c>
@@ -1178,56 +1221,60 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="0" t="n">
+      <c r="A25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="F25" s="0" t="n">
+      <c r="D25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>18743.8345746994</v>
-      </c>
-      <c r="I25" s="7" t="n">
-        <v>0.9884</v>
-      </c>
-      <c r="J25" s="7" t="n">
-        <v>0.9644</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="L25" s="7" t="n">
-        <v>0.9893</v>
-      </c>
-      <c r="M25" s="7" t="n">
-        <v>0.8998</v>
-      </c>
-      <c r="N25" s="0" t="n">
-        <v>20</v>
+      <c r="G25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="R25" s="0" t="s">
         <v>62</v>
       </c>
       <c r="S25" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -1240,28 +1287,28 @@
         <v>9</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>27534.1222834587</v>
+        <v>13888.2287483215</v>
       </c>
       <c r="I26" s="7" t="n">
-        <v>0.9943</v>
+        <v>0.9817</v>
       </c>
       <c r="J26" s="7" t="n">
-        <v>0.9564</v>
+        <v>0.9609</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>9</v>
       </c>
       <c r="L26" s="7" t="n">
-        <v>0.999</v>
+        <v>0.9887</v>
       </c>
       <c r="M26" s="7" t="n">
-        <v>0.9336</v>
+        <v>0.902</v>
       </c>
       <c r="N26" s="0" t="n">
         <v>20</v>
@@ -1270,12 +1317,14 @@
         <v>64</v>
       </c>
       <c r="S26" s="0" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="6"/>
       <c r="C27" s="0" t="n">
         <v>4</v>
       </c>
@@ -1286,34 +1335,220 @@
         <v>16</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="H27" s="0" t="n">
+        <v>18743.8345746994</v>
+      </c>
+      <c r="I27" s="7" t="n">
+        <v>0.9884</v>
+      </c>
+      <c r="J27" s="7" t="n">
+        <v>0.9644</v>
+      </c>
       <c r="K27" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="L27" s="7" t="n">
+        <v>0.9893</v>
+      </c>
+      <c r="M27" s="7" t="n">
+        <v>0.8998</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R27" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" s="7" t="n">
+        <v>0.9985</v>
+      </c>
+      <c r="J28" s="7" t="n">
+        <v>0.9607</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="L28" s="7" t="n">
+        <v>0.9986</v>
+      </c>
+      <c r="M28" s="7" t="n">
+        <v>0.9385</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="0" t="n">
+      <c r="A29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>27534.1222834587</v>
+      </c>
+      <c r="I29" s="7" t="n">
+        <v>0.9943</v>
+      </c>
+      <c r="J29" s="7" t="n">
+        <v>0.9564</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="L29" s="7" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="M29" s="7" t="n">
+        <v>0.9336</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="R29" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="S29" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>70000</v>
+      </c>
+      <c r="I30" s="7" t="n">
+        <v>0.9989</v>
+      </c>
+      <c r="J30" s="7" t="n">
+        <v>0.9659</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="L30" s="7" t="n">
+        <v>0.9993</v>
+      </c>
+      <c r="M30" s="7" t="n">
+        <v>0.9419</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J32" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="7" t="n">
+        <v>0.6602</v>
+      </c>
+      <c r="D40" s="7" t="n">
+        <v>0.5442</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="7" t="n">
+        <v>0.8262</v>
+      </c>
+      <c r="D41" s="7" t="n">
+        <v>0.6855</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H47" s="0" t="n">
         <f aca="false">SUM(H4:H8)/3600</f>
         <v>17.4515191955699</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
     <mergeCell ref="A1:N2"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="A22:N22"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="A24:N24"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Almost penultimate backup + adding readme et al.
</commit_message>
<xml_diff>
--- a/src/experiments/experiment_results.xlsx
+++ b/src/experiments/experiment_results.xlsx
@@ -458,7 +458,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -536,6 +536,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -642,8 +646,8 @@
   </sheetPr>
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1369,7 +1373,7 @@
       <c r="D19" s="17" t="n">
         <v>0.9998</v>
       </c>
-      <c r="E19" s="17" t="n">
+      <c r="E19" s="20" t="n">
         <v>0.9641</v>
       </c>
       <c r="F19" s="18" t="n">
@@ -1489,7 +1493,7 @@
       <c r="F22" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="21" t="s">
         <v>17</v>
       </c>
       <c r="H22" s="17" t="n">
@@ -1517,20 +1521,20 @@
         <v>62</v>
       </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="21" t="n">
+      <c r="D23" s="22" t="n">
         <v>0.9798</v>
       </c>
-      <c r="E23" s="21" t="n">
+      <c r="E23" s="22" t="n">
         <v>0.87</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21" t="n">
+      <c r="G23" s="21"/>
+      <c r="H23" s="22" t="n">
         <v>0.9998</v>
       </c>
-      <c r="I23" s="21" t="n">
+      <c r="I23" s="22" t="n">
         <v>0.9487</v>
       </c>
       <c r="J23" s="0" t="n">
@@ -1548,32 +1552,32 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="23" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="23" t="n">
+      <c r="D24" s="24" t="n">
         <v>0.9937</v>
       </c>
-      <c r="E24" s="23" t="n">
+      <c r="E24" s="24" t="n">
         <v>0.9384</v>
       </c>
-      <c r="F24" s="22" t="n">
+      <c r="F24" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="23" t="n">
+      <c r="G24" s="21"/>
+      <c r="H24" s="24" t="n">
         <v>0.9998</v>
       </c>
-      <c r="I24" s="23" t="n">
+      <c r="I24" s="24" t="n">
         <v>0.9789</v>
       </c>
-      <c r="J24" s="22" t="n">
-        <v>20</v>
-      </c>
-      <c r="K24" s="22" t="s">
+      <c r="J24" s="23" t="n">
+        <v>20</v>
+      </c>
+      <c r="K24" s="23" t="s">
         <v>65</v>
       </c>
       <c r="R24" s="0" t="s">
@@ -1684,19 +1688,19 @@
       <c r="H29" s="0" t="n">
         <v>13888.2287483215</v>
       </c>
-      <c r="I29" s="21" t="n">
+      <c r="I29" s="22" t="n">
         <v>0.9817</v>
       </c>
-      <c r="J29" s="21" t="n">
+      <c r="J29" s="22" t="n">
         <v>0.9609</v>
       </c>
       <c r="K29" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="L29" s="21" t="n">
+      <c r="L29" s="22" t="n">
         <v>0.9887</v>
       </c>
-      <c r="M29" s="21" t="n">
+      <c r="M29" s="22" t="n">
         <v>0.902</v>
       </c>
       <c r="N29" s="0" t="n">
@@ -1728,19 +1732,19 @@
       <c r="H30" s="0" t="n">
         <v>18743.8345746994</v>
       </c>
-      <c r="I30" s="21" t="n">
+      <c r="I30" s="22" t="n">
         <v>0.9884</v>
       </c>
-      <c r="J30" s="21" t="n">
+      <c r="J30" s="22" t="n">
         <v>0.9644</v>
       </c>
       <c r="K30" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="L30" s="21" t="n">
+      <c r="L30" s="22" t="n">
         <v>0.9893</v>
       </c>
-      <c r="M30" s="21" t="n">
+      <c r="M30" s="22" t="n">
         <v>0.8998</v>
       </c>
       <c r="N30" s="0" t="n">
@@ -1772,19 +1776,19 @@
       <c r="H31" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="I31" s="21" t="n">
+      <c r="I31" s="22" t="n">
         <v>0.9985</v>
       </c>
-      <c r="J31" s="21" t="n">
+      <c r="J31" s="22" t="n">
         <v>0.9607</v>
       </c>
       <c r="K31" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="L31" s="21" t="n">
+      <c r="L31" s="22" t="n">
         <v>0.9986</v>
       </c>
-      <c r="M31" s="21" t="n">
+      <c r="M31" s="22" t="n">
         <v>0.9385</v>
       </c>
       <c r="N31" s="0" t="n">
@@ -1816,19 +1820,19 @@
       <c r="H32" s="0" t="n">
         <v>9265.1885433197</v>
       </c>
-      <c r="I32" s="21" t="n">
+      <c r="I32" s="22" t="n">
         <v>0.9721</v>
       </c>
-      <c r="J32" s="21" t="n">
+      <c r="J32" s="22" t="n">
         <v>0.9555</v>
       </c>
       <c r="K32" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="L32" s="21" t="n">
+      <c r="L32" s="22" t="n">
         <v>0.9816</v>
       </c>
-      <c r="M32" s="21" t="n">
+      <c r="M32" s="22" t="n">
         <v>0.8825</v>
       </c>
       <c r="N32" s="0" t="n">
@@ -1860,19 +1864,19 @@
       <c r="H33" s="0" t="n">
         <v>27534.1222834587</v>
       </c>
-      <c r="I33" s="21" t="n">
+      <c r="I33" s="22" t="n">
         <v>0.9943</v>
       </c>
-      <c r="J33" s="21" t="n">
+      <c r="J33" s="22" t="n">
         <v>0.9564</v>
       </c>
       <c r="K33" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="L33" s="21" t="n">
+      <c r="L33" s="22" t="n">
         <v>0.999</v>
       </c>
-      <c r="M33" s="21" t="n">
+      <c r="M33" s="22" t="n">
         <v>0.9336</v>
       </c>
       <c r="N33" s="0" t="n">
@@ -1886,40 +1890,40 @@
       <c r="B34" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="22" t="n">
+      <c r="C34" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="D34" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="22" t="n">
+      <c r="D34" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="23" t="n">
         <v>16</v>
       </c>
-      <c r="F34" s="22" t="n">
+      <c r="F34" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="G34" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" s="22" t="n">
+      <c r="G34" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="23" t="n">
         <v>70000</v>
       </c>
-      <c r="I34" s="23" t="n">
+      <c r="I34" s="24" t="n">
         <v>0.9989</v>
       </c>
-      <c r="J34" s="23" t="n">
+      <c r="J34" s="24" t="n">
         <v>0.9659</v>
       </c>
-      <c r="K34" s="22" t="n">
+      <c r="K34" s="23" t="n">
         <v>16</v>
       </c>
-      <c r="L34" s="23" t="n">
+      <c r="L34" s="24" t="n">
         <v>0.9993</v>
       </c>
-      <c r="M34" s="23" t="n">
+      <c r="M34" s="24" t="n">
         <v>0.9428</v>
       </c>
-      <c r="N34" s="22" t="n">
+      <c r="N34" s="23" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1930,37 +1934,37 @@
       <c r="B35" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="24" t="n">
+      <c r="C35" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="D35" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E35" s="24" t="n">
+      <c r="D35" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="F35" s="24" t="n">
+      <c r="F35" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="G35" s="24" t="n">
+      <c r="G35" s="25" t="n">
         <v>1</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>50000</v>
       </c>
-      <c r="I35" s="21" t="n">
+      <c r="I35" s="22" t="n">
         <v>0.9892</v>
       </c>
-      <c r="J35" s="21" t="n">
+      <c r="J35" s="22" t="n">
         <v>0.9593</v>
       </c>
       <c r="K35" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="L35" s="21" t="n">
+      <c r="L35" s="22" t="n">
         <v>0.9987</v>
       </c>
-      <c r="M35" s="21" t="n">
+      <c r="M35" s="22" t="n">
         <v>0.9337</v>
       </c>
       <c r="N35" s="0" t="n">
@@ -1994,10 +1998,10 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="26" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="0" t="n">
@@ -2018,19 +2022,19 @@
       <c r="H37" s="0" t="n">
         <v>5783.84894371033</v>
       </c>
-      <c r="I37" s="21" t="n">
+      <c r="I37" s="22" t="n">
         <v>0.958</v>
       </c>
-      <c r="J37" s="21" t="n">
+      <c r="J37" s="22" t="n">
         <v>0.9405</v>
       </c>
       <c r="K37" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="L37" s="21" t="n">
+      <c r="L37" s="22" t="n">
         <v>0.9905</v>
       </c>
-      <c r="M37" s="21" t="n">
+      <c r="M37" s="22" t="n">
         <v>0.8803</v>
       </c>
       <c r="N37" s="0" t="n">
@@ -2041,10 +2045,10 @@
       <c r="B44" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="21" t="n">
+      <c r="C44" s="22" t="n">
         <v>0.6602</v>
       </c>
-      <c r="D44" s="21" t="n">
+      <c r="D44" s="22" t="n">
         <v>0.5442</v>
       </c>
       <c r="E44" s="0" t="s">
@@ -2055,10 +2059,10 @@
       <c r="B45" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="21" t="n">
+      <c r="C45" s="22" t="n">
         <v>0.8266</v>
       </c>
-      <c r="D45" s="21" t="n">
+      <c r="D45" s="22" t="n">
         <v>0.6956</v>
       </c>
       <c r="E45" s="0" t="s">

</xml_diff>